<commit_message>
[T] Update test to cover more cases
</commit_message>
<xml_diff>
--- a/tests/testdata/test_fas/fas_excel_test.xlsx
+++ b/tests/testdata/test_fas/fas_excel_test.xlsx
@@ -9,6 +9,7 @@
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Summary" sheetId="1" state="visible" r:id="rId1"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Data" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="HelloWorld" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -414,7 +415,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -423,18 +424,22 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Hello</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>World</t>
-        </is>
+      <c r="A1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B1" t="n">
+        <v>20</v>
+      </c>
+      <c r="C1">
+        <f>SUM(A1,B1)</f>
+        <v/>
       </c>
     </row>
+    <row r="2"/>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:B2"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -466,4 +471,35 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Hello</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>World</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
[T] Add more test cases for the new features of FAS excel. Update test file
</commit_message>
<xml_diff>
--- a/tests/testdata/test_fas/fas_excel_test.xlsx
+++ b/tests/testdata/test_fas/fas_excel_test.xlsx
@@ -124,6 +124,105 @@
     </indexedColors>
   </colors>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Sample Chart</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <barChart>
+        <barDir val="col"/>
+        <grouping val="clustered"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <spPr>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <val>
+            <numRef>
+              <f>'Data'!$A$1:$A$2</f>
+            </numRef>
+          </val>
+        </ser>
+        <gapWidth val="150"/>
+        <axId val="10"/>
+        <axId val="100"/>
+      </barChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>2</col>
+      <colOff>0</colOff>
+      <row>4</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="1" name="Chart 1"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -470,6 +569,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>